<commit_message>
Wrote code to update system using Alamouti coding and wrote new code for non-linear analysis
</commit_message>
<xml_diff>
--- a/Alamouti_AdapEq_Analysis.xlsx
+++ b/Alamouti_AdapEq_Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karun\Desktop\Engineering Tripos\IIB_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B714E298-E9C4-4EC4-B3A6-6B99A2AAD74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0B3494-0795-499B-929E-9A577D8BADAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="7" xr2:uid="{D2C83010-40A7-49C2-84BA-9DCEB78ECCE1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="13" xr2:uid="{D2C83010-40A7-49C2-84BA-9DCEB78ECCE1}"/>
   </bookViews>
   <sheets>
     <sheet name="InitialTest" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,12 @@
     <sheet name="Hermitian" sheetId="8" r:id="rId6"/>
     <sheet name="Only Training" sheetId="9" r:id="rId7"/>
     <sheet name="w22=-1" sheetId="10" r:id="rId8"/>
+    <sheet name="Rotations" sheetId="11" r:id="rId9"/>
+    <sheet name="Rotations+Phase Noise" sheetId="12" r:id="rId10"/>
+    <sheet name="Revisiting CD" sheetId="13" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="16" r:id="rId12"/>
+    <sheet name="Phase Noise -SpS=2" sheetId="14" r:id="rId13"/>
+    <sheet name="CDC" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="51">
   <si>
     <t>N1</t>
   </si>
@@ -104,11 +110,107 @@
   <si>
     <t>N/A</t>
   </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Errors are zero, but symbols haven't converged to a point</t>
+  </si>
+  <si>
+    <t>Non-zero errors for almost all rotations</t>
+  </si>
+  <si>
+    <t>Non-zero errors for about half of the rotations</t>
+  </si>
+  <si>
+    <t>Errors are zero, but there are four blobs around each original symbol location</t>
+  </si>
+  <si>
+    <t>Increasing number of symbols has allowed for better, yet unsatisfactory convergence into a  single blob</t>
+  </si>
+  <si>
+    <t>Errors are zero, but not a large change from before</t>
+  </si>
+  <si>
+    <t>Similar to the case above</t>
+  </si>
+  <si>
+    <t>Errors are zero, but we have messy blobs</t>
+  </si>
+  <si>
+    <t>Errors are zero, but slight reduction in convergence</t>
+  </si>
+  <si>
+    <t>Clouds are too big</t>
+  </si>
+  <si>
+    <t>w_22</t>
+  </si>
+  <si>
+    <t>Larger clouds than before</t>
+  </si>
+  <si>
+    <t>Slightly better</t>
+  </si>
+  <si>
+    <t>Errors are zero, except for 90; there is a significant cloud</t>
+  </si>
+  <si>
+    <t>Same as before, better convergence during training period only</t>
+  </si>
+  <si>
+    <t>Same  as before</t>
+  </si>
+  <si>
+    <t>Same as before for larger rotations. Worse for smaller rotations</t>
+  </si>
+  <si>
+    <t>error reduced for 90 but became non-zero for some others</t>
+  </si>
+  <si>
+    <t>Linewidth</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>Final symbols form lines through the original points</t>
+  </si>
+  <si>
+    <t>Thicker but shorter lines than before</t>
+  </si>
+  <si>
+    <t>Not that different to the previous case</t>
+  </si>
+  <si>
+    <t>Thicker, slighltly shorte lines than before</t>
+  </si>
+  <si>
+    <t>Larger blobs than lines</t>
+  </si>
+  <si>
+    <t>Reasonably good</t>
+  </si>
+  <si>
+    <t>Diverges at the end; Mu_T and DD too high</t>
+  </si>
+  <si>
+    <t>Relatively slow convergence</t>
+  </si>
+  <si>
+    <t>Amazing</t>
+  </si>
+  <si>
+    <t>SpS=2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -187,6 +289,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -805,6 +914,1511 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{619F6C84-6C8E-4AFD-9218-7A8C4385D65E}">
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+    <col min="13" max="13" width="53" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H2" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H3" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H5" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="I5" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="I6" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0.2465</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>2.4E-2</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D536BE8A-8C47-41D8-B676-8B2B5CE4DB2A}">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L2" s="9">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L3" s="9">
+        <v>9.3899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L4" s="9">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.1275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>480000</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.1216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="1">
+        <v>480000</v>
+      </c>
+      <c r="H7" s="8">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="I7" s="8">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.1052</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>480000</v>
+      </c>
+      <c r="H8" s="8">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="I8" s="8">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>20000000000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G12" s="1">
+        <v>480000</v>
+      </c>
+      <c r="H12" s="8">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="I12" s="8">
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.2233</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="I14" s="8">
+        <v>1.5999999999999999E-5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="L14" s="9">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G15" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1.45E-5</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1.45E-5</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="L15" s="9">
+        <v>2.5000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.3">
+      <c r="D19" s="10"/>
+      <c r="L19" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E5E707-8792-4ECE-886F-99EE4A46D9D9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58E89ED-D789-4DAB-ACE3-D9B0B25C1163}">
+  <dimension ref="A1:N13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="A1:N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" customWidth="1"/>
+    <col min="14" max="14" width="41.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8">
+        <v>10000</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J2" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="9"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H4" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J4" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>50</v>
+      </c>
+      <c r="C5" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H5" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J5" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>50</v>
+      </c>
+      <c r="C6" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H6" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>50</v>
+      </c>
+      <c r="C7" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H7" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>50</v>
+      </c>
+      <c r="C8" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H8" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1.7E-5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1.7E-5</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>50</v>
+      </c>
+      <c r="C9" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H9" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I9" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J9" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="K9" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H10" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J10" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="K10" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>50</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H12" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I12" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J12" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="K12" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>50</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1000000</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>75000</v>
+      </c>
+      <c r="H13" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0.15</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="9">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{403DA77F-6B80-43ED-8BBE-AD15E7972153}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" customWidth="1"/>
+    <col min="13" max="13" width="12.77734375" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H2" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="J2" s="8">
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.48230000000000001</v>
+      </c>
+      <c r="M2" s="9">
+        <v>4.1000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>50</v>
+      </c>
+      <c r="C3" s="8">
+        <v>100000</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>280000</v>
+      </c>
+      <c r="I3" s="8">
+        <v>2.3E-5</v>
+      </c>
+      <c r="J3" s="8">
+        <v>2.3E-5</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.48230000000000001</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.2477</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD67E1C-96CB-4837-8CD4-EECBB80FA4C6}">
   <dimension ref="A1:I23"/>
@@ -2518,7 +4132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA068002-B6DC-4147-9AE0-53BDEB2AB074}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection sqref="A1:N6"/>
     </sheetView>
   </sheetViews>
@@ -4592,8 +6206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710B6CE6-B0D6-4993-9BC3-CF692B817D95}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4809,4 +6423,638 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5363AB33-54D0-499D-9CF2-3627C012BBB1}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.21875" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="83.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B2" s="1">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H2" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="I2" s="8">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="J2" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B3" s="1">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H3" s="8">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="I3" s="8">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="J3" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G4" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B5" s="1">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G5" s="1">
+        <v>280000</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J5" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B6" s="1">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J6" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B7" s="1">
+        <v>50</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G7" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B8" s="1">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1">
+        <v>25</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G8" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B9" s="1">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G9" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J9" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B10" s="1">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>100000</v>
+      </c>
+      <c r="G10" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+      <c r="M10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B11" s="1">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="1">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>75000</v>
+      </c>
+      <c r="G11" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="1">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>75000</v>
+      </c>
+      <c r="G12" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="I12" s="8">
+        <v>1.5E-5</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1">
+        <v>25</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>75000</v>
+      </c>
+      <c r="G13" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1.1E-5</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1.1E-5</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B14" s="1">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>75000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1.2E-5</v>
+      </c>
+      <c r="I14" s="8">
+        <v>1.2E-5</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>50000000000</v>
+      </c>
+      <c r="B15" s="1">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="1">
+        <v>25</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>75000</v>
+      </c>
+      <c r="G15" s="1">
+        <v>380000</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1.2E-5</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1.2E-5</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>